<commit_message>
Update con diverse tabelle
</commit_message>
<xml_diff>
--- a/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_GL3.xlsx
+++ b/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_GL3.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Documents\GitHub\GDPRProject\Documentazione\GDPRPrj_TempiLavoro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\s128438\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E26725-4A25-4B9A-8D9B-9DC2D1B84FC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{93EB8B36-C556-4775-9097-F89B03EE0B0D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="34">
   <si>
     <t>Persona</t>
   </si>
@@ -117,13 +116,39 @@
   </si>
   <si>
     <t>Ore</t>
+  </si>
+  <si>
+    <t>ore di lavoro*</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">* ore </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>× persone</t>
+    </r>
+  </si>
+  <si>
+    <t>Totali per attività</t>
+  </si>
+  <si>
+    <t>Totali per progetto</t>
+  </si>
+  <si>
+    <t>Intenro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +187,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -433,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -472,6 +503,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -532,7 +564,24 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -846,11 +895,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A511A23-0AE1-43CE-B25D-50A28135284A}">
-  <dimension ref="B1:T56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,63 +908,109 @@
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:20" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="41" t="s">
+    <row r="1" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:26" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43"/>
-    </row>
-    <row r="3" spans="2:20" ht="24" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="44"/>
+    </row>
+    <row r="3" spans="2:26" ht="24" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
     </row>
-    <row r="4" spans="2:20" ht="21" x14ac:dyDescent="0.35">
-      <c r="B4" s="47" t="s">
+    <row r="4" spans="2:26" ht="21" x14ac:dyDescent="0.35">
+      <c r="B4" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="49"/>
-    </row>
-    <row r="5" spans="2:20" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="50" t="s">
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="58"/>
+      <c r="J4" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="50"/>
+      <c r="S4" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="T4" s="49"/>
+      <c r="U4" s="55"/>
+      <c r="V4" s="55"/>
+      <c r="W4" s="55"/>
+      <c r="X4" s="55"/>
+      <c r="Y4" s="55"/>
+      <c r="Z4" s="56"/>
+    </row>
+    <row r="5" spans="2:26" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="48"/>
+      <c r="C5" s="49"/>
       <c r="D5" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="50" t="s">
+      <c r="E5" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="51"/>
-      <c r="G5" s="52"/>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="44" t="s">
+      <c r="F5" s="52"/>
+      <c r="G5" s="53"/>
+      <c r="J5" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="60"/>
+      <c r="L5" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="O5" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="S5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B6" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="44"/>
+      <c r="C6" s="45"/>
       <c r="D6" s="10">
         <f>SUM(J14:J47)</f>
         <v>950</v>
@@ -924,16 +1019,30 @@
         <f t="shared" ref="E6:E9" si="0">_xlfn.FLOOR.MATH(D6/60)</f>
         <v>15</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="37"/>
-    </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="45" t="s">
+      <c r="G6" s="38"/>
+      <c r="J6" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="45"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="57"/>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="57"/>
+      <c r="S6" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="T6" s="57"/>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B7" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="45"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="7">
         <f>SUM(O14:O117)</f>
         <v>2850</v>
@@ -942,16 +1051,26 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="35"/>
-    </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="46" t="s">
+      <c r="G7" s="36"/>
+      <c r="J7" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="46"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="64"/>
+      <c r="N7" s="65"/>
+      <c r="O7" s="65"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B8" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="46"/>
+      <c r="C8" s="47"/>
       <c r="D8" s="26">
         <f>SUM(T14:T51)</f>
         <v>2490</v>
@@ -960,74 +1079,97 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="37"/>
-    </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="45" t="s">
+      <c r="G8" s="38"/>
+      <c r="J8" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="47"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="57"/>
+      <c r="O8" s="57"/>
+      <c r="P8" s="57"/>
+      <c r="Q8" s="57"/>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B9" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="45"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="7">
         <f>SUM(E14:E37)</f>
         <v>750</v>
       </c>
       <c r="E9" s="29">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="F9" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="35"/>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="53" t="s">
+        <f>_xlfn.FLOOR.MATH(D9/60)*3</f>
+        <v>36</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="36"/>
+      <c r="H9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="53"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="64"/>
+      <c r="N9" s="65"/>
+      <c r="O9" s="65"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B10" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="54"/>
       <c r="D10" s="27">
         <f>SUM(D6:D9)</f>
         <v>7040</v>
       </c>
       <c r="E10" s="28">
-        <f>_xlfn.FLOOR.MATH(D10/60)</f>
-        <v>117</v>
-      </c>
-      <c r="F10" s="36" t="s">
+        <f>SUM(E6:E9)</f>
+        <v>139</v>
+      </c>
+      <c r="F10" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="37"/>
-    </row>
-    <row r="12" spans="2:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="38" t="s">
+      <c r="G10" s="38"/>
+    </row>
+    <row r="12" spans="2:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B12" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="40"/>
-      <c r="G12" s="38" t="s">
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="41"/>
+      <c r="G12" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="40"/>
-      <c r="L12" s="38" t="s">
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="41"/>
+      <c r="L12" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="40"/>
-      <c r="Q12" s="38" t="s">
+      <c r="M12" s="40"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="41"/>
+      <c r="Q12" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="R12" s="39"/>
-      <c r="S12" s="39"/>
-      <c r="T12" s="40"/>
-    </row>
-    <row r="13" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R12" s="40"/>
+      <c r="S12" s="40"/>
+      <c r="T12" s="41"/>
+    </row>
+    <row r="13" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>1</v>
       </c>
@@ -1077,7 +1219,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
@@ -1127,7 +1269,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>5</v>
       </c>
@@ -1177,7 +1319,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
@@ -2266,26 +2408,34 @@
       </c>
     </row>
     <row r="56" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L56" s="54" t="s">
-        <v>5</v>
-      </c>
-      <c r="M56" s="54" t="s">
+      <c r="L56" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="M56" s="34" t="s">
         <v>16</v>
       </c>
       <c r="N56" s="33">
         <v>43577</v>
       </c>
-      <c r="O56" s="54">
+      <c r="O56" s="34">
         <v>120</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="Q12:T12"/>
+  <mergeCells count="25">
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J4:Q4"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
@@ -2293,12 +2443,11 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="Q12:T12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Inserito modello COCOMO + update tempi
</commit_message>
<xml_diff>
--- a/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_GL3.xlsx
+++ b/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_GL3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gianluca\Documents\GitHub\GDPRProject\Documentazione\GDPRPrj_TempiLavoro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E2A99C-02E9-4B16-A236-652BC5AB8D75}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2061EC-FC55-4763-9188-A769E7FEA446}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -472,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -523,22 +523,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -550,9 +580,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -562,36 +589,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -909,7 +911,7 @@
   <dimension ref="B1:Z56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,12 +935,12 @@
   <sheetData>
     <row r="1" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:26" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="66"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="2:26" ht="24" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B3" s="25"/>
@@ -947,29 +949,29 @@
       <c r="E3" s="25"/>
     </row>
     <row r="4" spans="2:26" ht="21" x14ac:dyDescent="0.35">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="51"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="38"/>
-      <c r="J4" s="46" t="s">
+      <c r="J4" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="51"/>
-      <c r="S4" s="46" t="s">
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="53"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="53"/>
+      <c r="P4" s="53"/>
+      <c r="Q4" s="54"/>
+      <c r="S4" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="T4" s="47"/>
+      <c r="T4" s="53"/>
       <c r="U4" s="35"/>
       <c r="V4" s="35"/>
       <c r="W4" s="35"/>
@@ -981,19 +983,19 @@
       <c r="B5" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="47"/>
+      <c r="C5" s="53"/>
       <c r="D5" s="30" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="56"/>
-      <c r="G5" s="57"/>
-      <c r="J5" s="48" t="s">
+      <c r="F5" s="65"/>
+      <c r="G5" s="66"/>
+      <c r="J5" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="49"/>
+      <c r="K5" s="61"/>
       <c r="L5" s="39" t="s">
         <v>12</v>
       </c>
@@ -1017,26 +1019,26 @@
       </c>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="50"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="10">
         <f>SUM(J14:J47)</f>
-        <v>1230</v>
+        <v>1290</v>
       </c>
       <c r="E6" s="28">
         <f t="shared" ref="E6:E8" si="0">_xlfn.FLOOR.MATH(D6/60)</f>
-        <v>20</v>
-      </c>
-      <c r="F6" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="60"/>
-      <c r="J6" s="50" t="s">
+      <c r="G6" s="59"/>
+      <c r="J6" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="50"/>
+      <c r="K6" s="49"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="37"/>
@@ -1049,10 +1051,10 @@
       <c r="T6" s="37"/>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="61"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="7">
         <f>SUM(O14:O117)</f>
         <v>2850</v>
@@ -1061,14 +1063,14 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="F7" s="67" t="s">
+      <c r="F7" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="68"/>
-      <c r="J7" s="61" t="s">
+      <c r="G7" s="57"/>
+      <c r="J7" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="61"/>
+      <c r="K7" s="50"/>
       <c r="L7" s="41"/>
       <c r="M7" s="41"/>
       <c r="N7" s="42"/>
@@ -1077,10 +1079,10 @@
       <c r="Q7" s="7"/>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="62"/>
+      <c r="C8" s="51"/>
       <c r="D8" s="26">
         <f>SUM(T14:T51)</f>
         <v>2490</v>
@@ -1089,14 +1091,14 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="60"/>
-      <c r="J8" s="62" t="s">
+      <c r="G8" s="59"/>
+      <c r="J8" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="62"/>
+      <c r="K8" s="51"/>
       <c r="L8" s="26"/>
       <c r="M8" s="10"/>
       <c r="N8" s="37"/>
@@ -1105,10 +1107,10 @@
       <c r="Q8" s="37"/>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="61"/>
+      <c r="C9" s="50"/>
       <c r="D9" s="7">
         <f>SUM(E14:E37)</f>
         <v>750</v>
@@ -1117,17 +1119,17 @@
         <f>_xlfn.FLOOR.MATH(D9/60)*3</f>
         <v>36</v>
       </c>
-      <c r="F9" s="67" t="s">
+      <c r="F9" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="68"/>
+      <c r="G9" s="57"/>
       <c r="H9" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="63" t="s">
+      <c r="J9" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="63"/>
+      <c r="K9" s="68"/>
       <c r="L9" s="43"/>
       <c r="M9" s="41"/>
       <c r="N9" s="42"/>
@@ -1136,48 +1138,48 @@
       <c r="Q9" s="7"/>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="58"/>
+      <c r="C10" s="67"/>
       <c r="D10" s="27">
         <f>SUM(D6:D9)</f>
-        <v>7320</v>
+        <v>7380</v>
       </c>
       <c r="E10" s="28">
         <f>SUM(E6:E9)</f>
-        <v>144</v>
-      </c>
-      <c r="F10" s="59" t="s">
+        <v>145</v>
+      </c>
+      <c r="F10" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="60"/>
+      <c r="G10" s="59"/>
     </row>
     <row r="12" spans="2:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="54"/>
-      <c r="G12" s="52" t="s">
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="64"/>
+      <c r="G12" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="54"/>
-      <c r="L12" s="52" t="s">
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="64"/>
+      <c r="L12" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="M12" s="53"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="54"/>
-      <c r="Q12" s="52" t="s">
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="64"/>
+      <c r="Q12" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="R12" s="53"/>
-      <c r="S12" s="53"/>
-      <c r="T12" s="54"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="64"/>
     </row>
     <row r="13" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
@@ -2160,17 +2162,17 @@
       </c>
     </row>
     <row r="35" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G35" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="H35" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="I35" s="33">
+      <c r="G35" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="I35" s="70">
         <v>43582</v>
       </c>
-      <c r="J35" s="34">
-        <v>60</v>
+      <c r="J35" s="69">
+        <v>120</v>
       </c>
       <c r="L35" s="4" t="s">
         <v>10</v>
@@ -2493,17 +2495,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F6:G6"/>
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J6:K6"/>
@@ -2518,6 +2509,17 @@
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="Q12:T12"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
TestR2 e update tempi
</commit_message>
<xml_diff>
--- a/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_GL3.xlsx
+++ b/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_GL3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gianluca\Documents\GitHub\GDPRProject\Documentazione\GDPRPrj_TempiLavoro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0810D3B1-9BE3-4FE1-BD3D-F027228B1A64}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D19A941-F97F-4B36-BA71-14E74BF7E945}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="34">
   <si>
     <t>Persona</t>
   </si>
@@ -527,52 +527,22 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -584,6 +554,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -593,7 +566,34 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -913,7 +913,7 @@
   <dimension ref="B1:Z56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,12 +937,12 @@
   <sheetData>
     <row r="1" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:26" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="52"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="70"/>
     </row>
     <row r="3" spans="2:26" ht="24" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B3" s="25"/>
@@ -951,29 +951,29 @@
       <c r="E3" s="25"/>
     </row>
     <row r="4" spans="2:26" ht="21" x14ac:dyDescent="0.35">
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="58"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="55"/>
       <c r="H4" s="38"/>
-      <c r="J4" s="56" t="s">
+      <c r="J4" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="58"/>
-      <c r="S4" s="56" t="s">
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="55"/>
+      <c r="S4" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="T4" s="57"/>
+      <c r="T4" s="51"/>
       <c r="U4" s="35"/>
       <c r="V4" s="35"/>
       <c r="W4" s="35"/>
@@ -985,19 +985,19 @@
       <c r="B5" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="57"/>
+      <c r="C5" s="51"/>
       <c r="D5" s="30" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="69"/>
-      <c r="G5" s="70"/>
-      <c r="J5" s="64" t="s">
+      <c r="F5" s="60"/>
+      <c r="G5" s="61"/>
+      <c r="J5" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="65"/>
+      <c r="K5" s="53"/>
       <c r="L5" s="39" t="s">
         <v>12</v>
       </c>
@@ -1021,26 +1021,26 @@
       </c>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="53"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="10">
         <f>SUM(J14:J47)</f>
-        <v>1440</v>
+        <v>1540</v>
       </c>
       <c r="E6" s="28">
         <f t="shared" ref="E6:E8" si="0">_xlfn.FLOOR.MATH(D6/60)</f>
-        <v>24</v>
-      </c>
-      <c r="F6" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="63"/>
-      <c r="J6" s="53" t="s">
+      <c r="G6" s="64"/>
+      <c r="J6" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="53"/>
+      <c r="K6" s="54"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="37"/>
@@ -1053,10 +1053,10 @@
       <c r="T6" s="37"/>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="54"/>
+      <c r="C7" s="65"/>
       <c r="D7" s="7">
         <f>SUM(O14:O117)</f>
         <v>2850</v>
@@ -1065,14 +1065,14 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="F7" s="60" t="s">
+      <c r="F7" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="61"/>
-      <c r="J7" s="54" t="s">
+      <c r="G7" s="72"/>
+      <c r="J7" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="54"/>
+      <c r="K7" s="65"/>
       <c r="L7" s="41"/>
       <c r="M7" s="41"/>
       <c r="N7" s="42"/>
@@ -1081,10 +1081,10 @@
       <c r="Q7" s="7"/>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="55"/>
+      <c r="C8" s="66"/>
       <c r="D8" s="26">
         <f>SUM(T14:T51)</f>
         <v>2490</v>
@@ -1093,14 +1093,14 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="F8" s="62" t="s">
+      <c r="F8" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="63"/>
-      <c r="J8" s="55" t="s">
+      <c r="G8" s="64"/>
+      <c r="J8" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="55"/>
+      <c r="K8" s="66"/>
       <c r="L8" s="26"/>
       <c r="M8" s="10"/>
       <c r="N8" s="37"/>
@@ -1109,10 +1109,10 @@
       <c r="Q8" s="37"/>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="54"/>
+      <c r="C9" s="65"/>
       <c r="D9" s="7">
         <f>SUM(E14:E37)</f>
         <v>750</v>
@@ -1121,17 +1121,17 @@
         <f>_xlfn.FLOOR.MATH(D9/60)*3</f>
         <v>36</v>
       </c>
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="61"/>
+      <c r="G9" s="72"/>
       <c r="H9" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="72" t="s">
+      <c r="J9" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="72"/>
+      <c r="K9" s="67"/>
       <c r="L9" s="43"/>
       <c r="M9" s="41"/>
       <c r="N9" s="42"/>
@@ -1140,48 +1140,48 @@
       <c r="Q9" s="7"/>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="71"/>
+      <c r="C10" s="62"/>
       <c r="D10" s="27">
         <f>SUM(D6:D9)</f>
-        <v>7530</v>
+        <v>7630</v>
       </c>
       <c r="E10" s="28">
         <f>SUM(E6:E9)</f>
-        <v>148</v>
-      </c>
-      <c r="F10" s="62" t="s">
+        <v>149</v>
+      </c>
+      <c r="F10" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="63"/>
+      <c r="G10" s="64"/>
     </row>
     <row r="12" spans="2:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="67"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="68"/>
-      <c r="G12" s="66" t="s">
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="58"/>
+      <c r="G12" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="68"/>
-      <c r="L12" s="66" t="s">
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="58"/>
+      <c r="L12" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="M12" s="67"/>
-      <c r="N12" s="67"/>
-      <c r="O12" s="68"/>
-      <c r="Q12" s="66" t="s">
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
+      <c r="O12" s="58"/>
+      <c r="Q12" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="R12" s="67"/>
-      <c r="S12" s="67"/>
-      <c r="T12" s="68"/>
+      <c r="R12" s="57"/>
+      <c r="S12" s="57"/>
+      <c r="T12" s="58"/>
     </row>
     <row r="13" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
@@ -2280,6 +2280,18 @@
       </c>
     </row>
     <row r="39" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H39" t="s">
+        <v>13</v>
+      </c>
+      <c r="I39" s="33">
+        <v>43584</v>
+      </c>
+      <c r="J39">
+        <v>40</v>
+      </c>
       <c r="L39" s="4" t="s">
         <v>5</v>
       </c>
@@ -2294,6 +2306,18 @@
       </c>
     </row>
     <row r="40" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>5</v>
+      </c>
+      <c r="H40" t="s">
+        <v>11</v>
+      </c>
+      <c r="I40" s="33">
+        <v>43584</v>
+      </c>
+      <c r="J40">
+        <v>60</v>
+      </c>
       <c r="L40" s="2" t="s">
         <v>5</v>
       </c>
@@ -2533,6 +2557,17 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J6:K6"/>
@@ -2547,17 +2582,6 @@
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="Q12:T12"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactoring parziale, commenti e update struttura TempiLavoro
</commit_message>
<xml_diff>
--- a/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_GL3.xlsx
+++ b/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_GL3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gianluca\Documents\GitHub\GDPRProject\Documentazione\GDPRPrj_TempiLavoro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Documenti\GitHub\GDPRProject\Documentazione\GDPRPrj_TempiLavoro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D19A941-F97F-4B36-BA71-14E74BF7E945}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BD0D9E-144B-460B-828A-06AF7224CB80}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="33">
   <si>
     <t>Persona</t>
   </si>
@@ -141,9 +141,6 @@
   </si>
   <si>
     <t>Totali per progetto</t>
-  </si>
-  <si>
-    <t>Intenro</t>
   </si>
 </sst>
 </file>
@@ -235,7 +232,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -468,11 +465,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -504,47 +527,64 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -554,9 +594,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -566,36 +603,44 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -912,278 +957,404 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="V38" sqref="V38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.88671875" customWidth="1"/>
+    <col min="21" max="21" width="13.44140625" customWidth="1"/>
+    <col min="22" max="22" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:26" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="68" t="s">
+    <row r="1" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:26" ht="24.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="70"/>
-    </row>
-    <row r="3" spans="2:26" ht="24" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37"/>
+    </row>
+    <row r="3" spans="2:26" ht="24" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
     </row>
-    <row r="4" spans="2:26" ht="21" x14ac:dyDescent="0.35">
-      <c r="B4" s="50" t="s">
+    <row r="4" spans="2:26" ht="21" x14ac:dyDescent="0.4">
+      <c r="B4" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="38"/>
-      <c r="J4" s="50" t="s">
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="33"/>
+      <c r="J4" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="55"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="43"/>
       <c r="S4" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="T4" s="51"/>
-      <c r="U4" s="35"/>
-      <c r="V4" s="35"/>
-      <c r="W4" s="35"/>
-      <c r="X4" s="35"/>
-      <c r="Y4" s="35"/>
-      <c r="Z4" s="36"/>
-    </row>
-    <row r="5" spans="2:26" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="59" t="s">
+      <c r="T4" s="50"/>
+      <c r="U4" s="50"/>
+      <c r="V4" s="50"/>
+      <c r="W4" s="33"/>
+      <c r="X4" s="33"/>
+      <c r="Y4" s="33"/>
+      <c r="Z4" s="33"/>
+    </row>
+    <row r="5" spans="2:26" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="30" t="s">
+      <c r="C5" s="42"/>
+      <c r="D5" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="60"/>
-      <c r="G5" s="61"/>
-      <c r="J5" s="52" t="s">
+      <c r="F5" s="54"/>
+      <c r="G5" s="55"/>
+      <c r="J5" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="53"/>
-      <c r="L5" s="39" t="s">
+      <c r="K5" s="50"/>
+      <c r="L5" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="N5" s="39" t="s">
+      <c r="M5" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="O5" s="40" t="s">
+      <c r="O5" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="P5" s="40" t="s">
+      <c r="P5" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="Q5" s="40" t="s">
+      <c r="Q5" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="S5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B6" s="54" t="s">
+      <c r="R5" s="64"/>
+      <c r="S5" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="T5" s="50"/>
+      <c r="U5" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="V5" s="65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B6" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="54"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="10">
         <f>SUM(J14:J47)</f>
         <v>1540</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="27">
         <f t="shared" ref="E6:E8" si="0">_xlfn.FLOOR.MATH(D6/60)</f>
         <v>25</v>
       </c>
-      <c r="F6" s="63" t="s">
+      <c r="F6" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="64"/>
-      <c r="J6" s="54" t="s">
+      <c r="G6" s="48"/>
+      <c r="J6" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="54"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37"/>
-      <c r="S6" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="T6" s="37"/>
-    </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B7" s="65" t="s">
+      <c r="K6" s="38"/>
+      <c r="L6" s="66">
+        <f>SUMIF(H14:H47,"CM",J14:J47)</f>
+        <v>120</v>
+      </c>
+      <c r="M6" s="66">
+        <f>SUMIF(H14:H47,"Documentazione",J14:J47)</f>
+        <v>1030</v>
+      </c>
+      <c r="N6" s="66">
+        <f>SUMIF(H14:H47,"Ricerche",J14:J47)</f>
+        <v>120</v>
+      </c>
+      <c r="O6" s="66">
+        <f>SUMIF(H14:H47,"Codice",J14:J47)</f>
+        <v>150</v>
+      </c>
+      <c r="P6" s="66">
+        <f>SUMIF(H14:H47,_xlnm.Database,J14:J47)</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="66">
+        <f>SUMIF(H14:H47,"Test",J14:J47)</f>
+        <v>120</v>
+      </c>
+      <c r="S6" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="T6" s="38"/>
+      <c r="U6" s="10">
+        <f>SUMIF(G14:G48,"Interno",J14:J48)</f>
+        <v>240</v>
+      </c>
+      <c r="V6" s="10">
+        <f>SUMIF(G14:G48,"GDPR",J14:J48)</f>
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B7" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="65"/>
+      <c r="C7" s="39"/>
       <c r="D7" s="7">
         <f>SUM(O14:O117)</f>
         <v>2850</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="28">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="F7" s="71" t="s">
+      <c r="F7" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="72"/>
-      <c r="J7" s="65" t="s">
+      <c r="G7" s="46"/>
+      <c r="J7" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="65"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="42"/>
-      <c r="O7" s="42"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-    </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B8" s="66" t="s">
+      <c r="K7" s="39"/>
+      <c r="L7" s="67">
+        <f>SUMIF(M14:M65,"CM",O14:O65)</f>
+        <v>340</v>
+      </c>
+      <c r="M7" s="67">
+        <f>SUMIF(M14:M65,"Documentazione",O14:O65)</f>
+        <v>970</v>
+      </c>
+      <c r="N7" s="67">
+        <f>SUMIF(M14:M65,"Ricerche",O14:O65)</f>
+        <v>90</v>
+      </c>
+      <c r="O7" s="67">
+        <f>SUMIF(M14:M65,"Codice",O14:O65)</f>
+        <v>1160</v>
+      </c>
+      <c r="P7" s="67">
+        <f>SUMIF(M14:M65,"Database",O14:O65)</f>
+        <v>290</v>
+      </c>
+      <c r="Q7" s="67">
+        <f>SUMIF(M14:M65,"Test",O14:O65)</f>
+        <v>0</v>
+      </c>
+      <c r="S7" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="T7" s="39"/>
+      <c r="U7" s="7">
+        <f>SUMIF(L14:L68,"Interno",O14:O68)</f>
+        <v>400</v>
+      </c>
+      <c r="V7" s="7">
+        <f>SUMIF(L14:L65,"GDPR",O14:O65)</f>
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B8" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="66"/>
+      <c r="C8" s="40"/>
       <c r="D8" s="26">
         <f>SUM(T14:T51)</f>
-        <v>2490</v>
-      </c>
-      <c r="E8" s="28">
+        <v>2715</v>
+      </c>
+      <c r="E8" s="27">
         <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="F8" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="64"/>
-      <c r="J8" s="66" t="s">
+      <c r="G8" s="48"/>
+      <c r="J8" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="66"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="37"/>
-    </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B9" s="65" t="s">
+      <c r="K8" s="40"/>
+      <c r="L8" s="66">
+        <f>SUMIF(R14:R47,"CM",T14:T47)</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="66">
+        <f>SUMIF(R14:R47,"Documentazione",T14:T47)</f>
+        <v>945</v>
+      </c>
+      <c r="N8" s="66">
+        <f>SUMIF(R14:R47,"Ricerche",T14:T47)</f>
+        <v>300</v>
+      </c>
+      <c r="O8" s="66">
+        <f>SUMIF(R14:R47,"Codice",T14:T47)</f>
+        <v>1200</v>
+      </c>
+      <c r="P8" s="66">
+        <f>SUMIF(R14:R47,"Database",T14:T47)</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="66">
+        <f>SUMIF(R14:R47,"Test",T14:T47)</f>
+        <v>0</v>
+      </c>
+      <c r="S8" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="T8" s="40"/>
+      <c r="U8" s="10">
+        <f>SUMIF(Q14:Q48,"Interno",T14:T48)</f>
+        <v>0</v>
+      </c>
+      <c r="V8" s="10">
+        <f>SUMIF(Q14:Q48,"GDPR",T14:T48)</f>
+        <v>2715</v>
+      </c>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B9" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="65"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="7">
         <f>SUM(E14:E37)</f>
         <v>750</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="28">
         <f>_xlfn.FLOOR.MATH(D9/60)*3</f>
         <v>36</v>
       </c>
-      <c r="F9" s="71" t="s">
+      <c r="F9" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="72"/>
+      <c r="G9" s="46"/>
       <c r="H9" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="67" t="s">
+      <c r="J9" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="67"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="42"/>
-      <c r="O9" s="42"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-    </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B10" s="62" t="s">
+      <c r="K9" s="57"/>
+      <c r="L9" s="68">
+        <f>SUMIF(H17:H50,"CM",J17:J50)</f>
+        <v>120</v>
+      </c>
+      <c r="M9" s="68">
+        <f>SUM(M6:M8)</f>
+        <v>2945</v>
+      </c>
+      <c r="N9" s="68">
+        <f>SUM(N6:N8)</f>
+        <v>510</v>
+      </c>
+      <c r="O9" s="68">
+        <f>SUM(O6:O8)</f>
+        <v>2510</v>
+      </c>
+      <c r="P9" s="69">
+        <f>SUM(P6:P8)</f>
+        <v>290</v>
+      </c>
+      <c r="Q9" s="69">
+        <f>SUM(Q6:Q8)</f>
+        <v>120</v>
+      </c>
+      <c r="S9" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="27">
+      <c r="T9" s="57"/>
+      <c r="U9" s="62">
+        <f>SUM(U6:U8)</f>
+        <v>640</v>
+      </c>
+      <c r="V9" s="62">
+        <f>SUM(V6:V8)</f>
+        <v>6465</v>
+      </c>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B10" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="56"/>
+      <c r="D10" s="70">
         <f>SUM(D6:D9)</f>
-        <v>7630</v>
-      </c>
-      <c r="E10" s="28">
+        <v>7855</v>
+      </c>
+      <c r="E10" s="70">
         <f>SUM(E6:E9)</f>
-        <v>149</v>
-      </c>
-      <c r="F10" s="63" t="s">
+        <v>153</v>
+      </c>
+      <c r="F10" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="64"/>
-    </row>
-    <row r="12" spans="2:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="56" t="s">
+      <c r="G10" s="72"/>
+    </row>
+    <row r="12" spans="2:26" ht="18" x14ac:dyDescent="0.35">
+      <c r="B12" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="58"/>
-      <c r="G12" s="56" t="s">
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="53"/>
+      <c r="G12" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="58"/>
-      <c r="L12" s="56" t="s">
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="53"/>
+      <c r="L12" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="M12" s="57"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="58"/>
-      <c r="Q12" s="56" t="s">
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="53"/>
+      <c r="Q12" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="R12" s="57"/>
-      <c r="S12" s="57"/>
-      <c r="T12" s="58"/>
-    </row>
-    <row r="13" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R12" s="52"/>
+      <c r="S12" s="52"/>
+      <c r="T12" s="53"/>
+    </row>
+    <row r="13" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
         <v>1</v>
       </c>
@@ -1233,7 +1404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
@@ -1283,7 +1454,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>5</v>
       </c>
@@ -1333,7 +1504,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
@@ -1383,7 +1554,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
@@ -1433,7 +1604,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
@@ -1483,7 +1654,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
@@ -1533,7 +1704,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>5</v>
       </c>
@@ -1583,7 +1754,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
         <v>5</v>
       </c>
@@ -1633,7 +1804,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
@@ -1683,7 +1854,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>5</v>
       </c>
@@ -1733,7 +1904,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>5</v>
       </c>
@@ -1783,7 +1954,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G25" s="4" t="s">
         <v>5</v>
       </c>
@@ -1821,7 +1992,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G26" s="2" t="s">
         <v>10</v>
       </c>
@@ -1859,7 +2030,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G27" s="4" t="s">
         <v>5</v>
       </c>
@@ -1897,7 +2068,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G28" s="2" t="s">
         <v>5</v>
       </c>
@@ -1935,7 +2106,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G29" s="4" t="s">
         <v>5</v>
       </c>
@@ -1973,7 +2144,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G30" s="2" t="s">
         <v>5</v>
       </c>
@@ -2011,17 +2182,17 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="G31" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="H31" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="I31" s="33">
+    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="G31" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" s="32">
         <v>43567</v>
       </c>
-      <c r="J31" s="32">
+      <c r="J31" s="31">
         <v>60</v>
       </c>
       <c r="L31" s="4" t="s">
@@ -2049,17 +2220,17 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="G32" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="H32" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="I32" s="33">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="G32" s="61" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="61" t="s">
+        <v>11</v>
+      </c>
+      <c r="I32" s="8">
         <v>43571</v>
       </c>
-      <c r="J32" s="34">
+      <c r="J32" s="61">
         <v>40</v>
       </c>
       <c r="L32" s="2" t="s">
@@ -2087,17 +2258,17 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G33" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="H33" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="I33" s="45">
+    <row r="33" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G33" s="73" t="s">
+        <v>5</v>
+      </c>
+      <c r="H33" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33" s="74">
         <v>43578</v>
       </c>
-      <c r="J33" s="44">
+      <c r="J33" s="73">
         <v>60</v>
       </c>
       <c r="L33" s="4" t="s">
@@ -2125,17 +2296,17 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I34" s="3">
+    <row r="34" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G34" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="H34" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="I34" s="59">
         <v>43581</v>
       </c>
-      <c r="J34" s="2">
+      <c r="J34" s="58">
         <v>60</v>
       </c>
       <c r="L34" s="2" t="s">
@@ -2160,20 +2331,20 @@
         <v>43567</v>
       </c>
       <c r="T34" s="10">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G35" s="46" t="s">
-        <v>5</v>
-      </c>
-      <c r="H35" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="I35" s="47">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G35" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="I35" s="14">
         <v>43582</v>
       </c>
-      <c r="J35" s="46">
+      <c r="J35" s="60">
         <v>120</v>
       </c>
       <c r="L35" s="4" t="s">
@@ -2194,24 +2365,24 @@
       <c r="R35" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="S35" s="31">
+      <c r="S35" s="30">
         <v>43569</v>
       </c>
       <c r="T35" s="13">
         <v>240</v>
       </c>
     </row>
-    <row r="36" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G36" s="48" t="s">
+    <row r="36" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G36" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H36" s="48" t="s">
+      <c r="H36" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I36" s="49">
+      <c r="I36" s="11">
         <v>43582</v>
       </c>
-      <c r="J36" s="48">
+      <c r="J36" s="10">
         <v>30</v>
       </c>
       <c r="L36" s="2" t="s">
@@ -2226,18 +2397,30 @@
       <c r="O36" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G37" t="s">
-        <v>5</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="Q36" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="R36" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="S36" s="11">
+        <v>43585</v>
+      </c>
+      <c r="T36" s="10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G37" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H37" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I37" s="33">
+      <c r="I37" s="8">
         <v>43583</v>
       </c>
-      <c r="J37">
+      <c r="J37" s="7">
         <v>50</v>
       </c>
       <c r="L37" s="4" t="s">
@@ -2252,18 +2435,30 @@
       <c r="O37" s="4">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G38" t="s">
-        <v>5</v>
-      </c>
-      <c r="H38" t="s">
-        <v>11</v>
-      </c>
-      <c r="I38" s="33">
+      <c r="Q37" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="R37" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="S37" s="8">
+        <v>43585</v>
+      </c>
+      <c r="T37" s="13">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G38" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" s="11">
         <v>43583</v>
       </c>
-      <c r="J38">
+      <c r="J38" s="10">
         <v>70</v>
       </c>
       <c r="L38" s="2" t="s">
@@ -2279,17 +2474,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G39" t="s">
-        <v>5</v>
-      </c>
-      <c r="H39" t="s">
+    <row r="39" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G39" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H39" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I39" s="33">
+      <c r="I39" s="8">
         <v>43584</v>
       </c>
-      <c r="J39">
+      <c r="J39" s="7">
         <v>40</v>
       </c>
       <c r="L39" s="4" t="s">
@@ -2305,17 +2500,17 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G40" t="s">
-        <v>5</v>
-      </c>
-      <c r="H40" t="s">
-        <v>11</v>
-      </c>
-      <c r="I40" s="33">
+    <row r="40" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G40" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I40" s="11">
         <v>43584</v>
       </c>
-      <c r="J40">
+      <c r="J40" s="10">
         <v>60</v>
       </c>
       <c r="L40" s="2" t="s">
@@ -2331,7 +2526,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L41" s="4" t="s">
         <v>5</v>
       </c>
@@ -2345,7 +2540,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L42" s="2" t="s">
         <v>5</v>
       </c>
@@ -2359,7 +2554,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L43" s="4" t="s">
         <v>5</v>
       </c>
@@ -2373,7 +2568,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L44" s="2" t="s">
         <v>5</v>
       </c>
@@ -2387,7 +2582,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L45" s="4" t="s">
         <v>5</v>
       </c>
@@ -2401,7 +2596,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L46" s="2" t="s">
         <v>5</v>
       </c>
@@ -2415,7 +2610,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L47" s="4" t="s">
         <v>5</v>
       </c>
@@ -2429,7 +2624,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L48" s="2" t="s">
         <v>5</v>
       </c>
@@ -2443,7 +2638,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="49" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L49" s="4" t="s">
         <v>10</v>
       </c>
@@ -2457,7 +2652,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L50" s="2" t="s">
         <v>5</v>
       </c>
@@ -2471,7 +2666,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L51" s="4" t="s">
         <v>5</v>
       </c>
@@ -2485,7 +2680,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L52" s="2" t="s">
         <v>5</v>
       </c>
@@ -2499,7 +2694,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L53" s="4" t="s">
         <v>5</v>
       </c>
@@ -2513,7 +2708,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L54" s="2" t="s">
         <v>5</v>
       </c>
@@ -2527,48 +2722,40 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L55" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="M55" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="N55" s="33">
+    <row r="55" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L55" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="M55" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="N55" s="32">
         <v>43577</v>
       </c>
-      <c r="O55" s="32">
+      <c r="O55" s="31">
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L56" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="M56" s="34" t="s">
+    <row r="56" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L56" s="61" t="s">
+        <v>5</v>
+      </c>
+      <c r="M56" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="N56" s="33">
+      <c r="N56" s="11">
         <v>43577</v>
       </c>
-      <c r="O56" s="34">
+      <c r="O56" s="61">
         <v>120</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="S4:T4"/>
+  <mergeCells count="30">
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="S4:V4"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="J4:Q4"/>
@@ -2582,6 +2769,19 @@
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="Q12:T12"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix notif e riorganizzazione
</commit_message>
<xml_diff>
--- a/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_GL3.xlsx
+++ b/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_GL3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Documenti\GitHub\GDPRProject\Documentazione\GDPRPrj_TempiLavoro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BD0D9E-144B-460B-828A-06AF7224CB80}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01C28D9-A08F-424F-AE0A-7A5DE7123CAA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="33">
   <si>
     <t>Persona</t>
   </si>
@@ -495,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -537,75 +537,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -633,14 +564,85 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -957,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="V38" sqref="V38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="T41" sqref="T41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -984,12 +986,12 @@
   <sheetData>
     <row r="1" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:26" ht="24.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="37"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="58"/>
     </row>
     <row r="3" spans="2:26" ht="24" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B3" s="25"/>
@@ -998,53 +1000,53 @@
       <c r="E3" s="25"/>
     </row>
     <row r="4" spans="2:26" ht="21" x14ac:dyDescent="0.4">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="43"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="62"/>
       <c r="H4" s="33"/>
-      <c r="J4" s="41" t="s">
+      <c r="J4" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="43"/>
-      <c r="S4" s="50" t="s">
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="62"/>
+      <c r="S4" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="T4" s="50"/>
-      <c r="U4" s="50"/>
-      <c r="V4" s="50"/>
+      <c r="T4" s="75"/>
+      <c r="U4" s="75"/>
+      <c r="V4" s="75"/>
       <c r="W4" s="33"/>
       <c r="X4" s="33"/>
       <c r="Y4" s="33"/>
       <c r="Z4" s="33"/>
     </row>
     <row r="5" spans="2:26" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="42"/>
+      <c r="C5" s="61"/>
       <c r="D5" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="44" t="s">
+      <c r="E5" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="54"/>
-      <c r="G5" s="55"/>
-      <c r="J5" s="49" t="s">
+      <c r="F5" s="68"/>
+      <c r="G5" s="69"/>
+      <c r="J5" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="50"/>
+      <c r="K5" s="75"/>
       <c r="L5" s="34" t="s">
         <v>12</v>
       </c>
@@ -1054,32 +1056,32 @@
       <c r="N5" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="O5" s="63" t="s">
+      <c r="O5" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="P5" s="63" t="s">
+      <c r="P5" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="Q5" s="63" t="s">
+      <c r="Q5" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="R5" s="64"/>
-      <c r="S5" s="49" t="s">
+      <c r="R5" s="41"/>
+      <c r="S5" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="T5" s="50"/>
-      <c r="U5" s="65" t="s">
+      <c r="T5" s="75"/>
+      <c r="U5" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="V5" s="65" t="s">
+      <c r="V5" s="42" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="38"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="10">
         <f>SUM(J14:J47)</f>
         <v>1540</v>
@@ -1088,42 +1090,42 @@
         <f t="shared" ref="E6:E8" si="0">_xlfn.FLOOR.MATH(D6/60)</f>
         <v>25</v>
       </c>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="48"/>
-      <c r="J6" s="38" t="s">
+      <c r="G6" s="67"/>
+      <c r="J6" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="38"/>
-      <c r="L6" s="66">
+      <c r="K6" s="54"/>
+      <c r="L6" s="43">
         <f>SUMIF(H14:H47,"CM",J14:J47)</f>
         <v>120</v>
       </c>
-      <c r="M6" s="66">
+      <c r="M6" s="43">
         <f>SUMIF(H14:H47,"Documentazione",J14:J47)</f>
         <v>1030</v>
       </c>
-      <c r="N6" s="66">
+      <c r="N6" s="43">
         <f>SUMIF(H14:H47,"Ricerche",J14:J47)</f>
         <v>120</v>
       </c>
-      <c r="O6" s="66">
+      <c r="O6" s="43">
         <f>SUMIF(H14:H47,"Codice",J14:J47)</f>
         <v>150</v>
       </c>
-      <c r="P6" s="66">
+      <c r="P6" s="43">
         <f>SUMIF(H14:H47,_xlnm.Database,J14:J47)</f>
         <v>0</v>
       </c>
-      <c r="Q6" s="66">
+      <c r="Q6" s="43">
         <f>SUMIF(H14:H47,"Test",J14:J47)</f>
         <v>120</v>
       </c>
-      <c r="S6" s="38" t="s">
+      <c r="S6" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="T6" s="38"/>
+      <c r="T6" s="54"/>
       <c r="U6" s="10">
         <f>SUMIF(G14:G48,"Interno",J14:J48)</f>
         <v>240</v>
@@ -1134,10 +1136,10 @@
       </c>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="39"/>
+      <c r="C7" s="55"/>
       <c r="D7" s="7">
         <f>SUM(O14:O117)</f>
         <v>2850</v>
@@ -1146,42 +1148,42 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="F7" s="45" t="s">
+      <c r="F7" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="46"/>
-      <c r="J7" s="39" t="s">
+      <c r="G7" s="65"/>
+      <c r="J7" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="39"/>
-      <c r="L7" s="67">
+      <c r="K7" s="55"/>
+      <c r="L7" s="44">
         <f>SUMIF(M14:M65,"CM",O14:O65)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="67">
+      <c r="M7" s="44">
         <f>SUMIF(M14:M65,"Documentazione",O14:O65)</f>
         <v>970</v>
       </c>
-      <c r="N7" s="67">
+      <c r="N7" s="44">
         <f>SUMIF(M14:M65,"Ricerche",O14:O65)</f>
         <v>90</v>
       </c>
-      <c r="O7" s="67">
+      <c r="O7" s="44">
         <f>SUMIF(M14:M65,"Codice",O14:O65)</f>
         <v>1160</v>
       </c>
-      <c r="P7" s="67">
+      <c r="P7" s="44">
         <f>SUMIF(M14:M65,"Database",O14:O65)</f>
         <v>290</v>
       </c>
-      <c r="Q7" s="67">
+      <c r="Q7" s="44">
         <f>SUMIF(M14:M65,"Test",O14:O65)</f>
         <v>0</v>
       </c>
-      <c r="S7" s="39" t="s">
+      <c r="S7" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="T7" s="39"/>
+      <c r="T7" s="55"/>
       <c r="U7" s="7">
         <f>SUMIF(L14:L68,"Interno",O14:O68)</f>
         <v>400</v>
@@ -1192,68 +1194,68 @@
       </c>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="40"/>
+      <c r="C8" s="59"/>
       <c r="D8" s="26">
         <f>SUM(T14:T51)</f>
-        <v>2715</v>
+        <v>2820</v>
       </c>
       <c r="E8" s="27">
         <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="F8" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="48"/>
-      <c r="J8" s="40" t="s">
+      <c r="G8" s="67"/>
+      <c r="J8" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="40"/>
-      <c r="L8" s="66">
+      <c r="K8" s="59"/>
+      <c r="L8" s="43">
         <f>SUMIF(R14:R47,"CM",T14:T47)</f>
         <v>0</v>
       </c>
-      <c r="M8" s="66">
+      <c r="M8" s="43">
         <f>SUMIF(R14:R47,"Documentazione",T14:T47)</f>
         <v>945</v>
       </c>
-      <c r="N8" s="66">
+      <c r="N8" s="43">
         <f>SUMIF(R14:R47,"Ricerche",T14:T47)</f>
         <v>300</v>
       </c>
-      <c r="O8" s="66">
+      <c r="O8" s="43">
         <f>SUMIF(R14:R47,"Codice",T14:T47)</f>
-        <v>1200</v>
-      </c>
-      <c r="P8" s="66">
+        <v>1260</v>
+      </c>
+      <c r="P8" s="43">
         <f>SUMIF(R14:R47,"Database",T14:T47)</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="66">
+      <c r="Q8" s="43">
         <f>SUMIF(R14:R47,"Test",T14:T47)</f>
-        <v>0</v>
-      </c>
-      <c r="S8" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="S8" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="T8" s="40"/>
+      <c r="T8" s="59"/>
       <c r="U8" s="10">
         <f>SUMIF(Q14:Q48,"Interno",T14:T48)</f>
         <v>0</v>
       </c>
       <c r="V8" s="10">
         <f>SUMIF(Q14:Q48,"GDPR",T14:T48)</f>
-        <v>2715</v>
+        <v>2820</v>
       </c>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="39"/>
+      <c r="C9" s="55"/>
       <c r="D9" s="7">
         <f>SUM(E14:E37)</f>
         <v>750</v>
@@ -1262,66 +1264,66 @@
         <f>_xlfn.FLOOR.MATH(D9/60)*3</f>
         <v>36</v>
       </c>
-      <c r="F9" s="45" t="s">
+      <c r="F9" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="46"/>
+      <c r="G9" s="65"/>
       <c r="H9" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="57" t="s">
+      <c r="J9" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="57"/>
-      <c r="L9" s="68">
+      <c r="K9" s="73"/>
+      <c r="L9" s="45">
         <f>SUMIF(H17:H50,"CM",J17:J50)</f>
         <v>120</v>
       </c>
-      <c r="M9" s="68">
+      <c r="M9" s="45">
         <f>SUM(M6:M8)</f>
         <v>2945</v>
       </c>
-      <c r="N9" s="68">
+      <c r="N9" s="45">
         <f>SUM(N6:N8)</f>
         <v>510</v>
       </c>
-      <c r="O9" s="68">
+      <c r="O9" s="45">
         <f>SUM(O6:O8)</f>
-        <v>2510</v>
-      </c>
-      <c r="P9" s="69">
+        <v>2570</v>
+      </c>
+      <c r="P9" s="46">
         <f>SUM(P6:P8)</f>
         <v>290</v>
       </c>
-      <c r="Q9" s="69">
+      <c r="Q9" s="46">
         <f>SUM(Q6:Q8)</f>
-        <v>120</v>
-      </c>
-      <c r="S9" s="57" t="s">
+        <v>165</v>
+      </c>
+      <c r="S9" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="T9" s="57"/>
-      <c r="U9" s="62">
+      <c r="T9" s="73"/>
+      <c r="U9" s="39">
         <f>SUM(U6:U8)</f>
         <v>640</v>
       </c>
-      <c r="V9" s="62">
+      <c r="V9" s="39">
         <f>SUM(V6:V8)</f>
-        <v>6465</v>
+        <v>6570</v>
       </c>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="70">
+      <c r="C10" s="70"/>
+      <c r="D10" s="47">
         <f>SUM(D6:D9)</f>
-        <v>7855</v>
-      </c>
-      <c r="E10" s="70">
+        <v>7960</v>
+      </c>
+      <c r="E10" s="47">
         <f>SUM(E6:E9)</f>
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F10" s="71" t="s">
         <v>26</v>
@@ -2221,16 +2223,16 @@
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="G32" s="61" t="s">
-        <v>5</v>
-      </c>
-      <c r="H32" s="61" t="s">
+      <c r="G32" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="38" t="s">
         <v>11</v>
       </c>
       <c r="I32" s="8">
         <v>43571</v>
       </c>
-      <c r="J32" s="61">
+      <c r="J32" s="38">
         <v>40</v>
       </c>
       <c r="L32" s="2" t="s">
@@ -2259,16 +2261,16 @@
       </c>
     </row>
     <row r="33" spans="7:20" x14ac:dyDescent="0.3">
-      <c r="G33" s="73" t="s">
-        <v>5</v>
-      </c>
-      <c r="H33" s="73" t="s">
-        <v>11</v>
-      </c>
-      <c r="I33" s="74">
+      <c r="G33" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="H33" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33" s="49">
         <v>43578</v>
       </c>
-      <c r="J33" s="73">
+      <c r="J33" s="48">
         <v>60</v>
       </c>
       <c r="L33" s="4" t="s">
@@ -2297,16 +2299,16 @@
       </c>
     </row>
     <row r="34" spans="7:20" x14ac:dyDescent="0.3">
-      <c r="G34" s="58" t="s">
-        <v>5</v>
-      </c>
-      <c r="H34" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="I34" s="59">
+      <c r="G34" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="H34" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="I34" s="36">
         <v>43581</v>
       </c>
-      <c r="J34" s="58">
+      <c r="J34" s="35">
         <v>60</v>
       </c>
       <c r="L34" s="2" t="s">
@@ -2335,16 +2337,16 @@
       </c>
     </row>
     <row r="35" spans="7:20" x14ac:dyDescent="0.3">
-      <c r="G35" s="60" t="s">
-        <v>5</v>
-      </c>
-      <c r="H35" s="60" t="s">
+      <c r="G35" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35" s="37" t="s">
         <v>11</v>
       </c>
       <c r="I35" s="14">
         <v>43582</v>
       </c>
-      <c r="J35" s="60">
+      <c r="J35" s="37">
         <v>120</v>
       </c>
       <c r="L35" s="4" t="s">
@@ -2473,6 +2475,18 @@
       <c r="O38" s="2">
         <v>10</v>
       </c>
+      <c r="Q38" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="R38" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="S38" s="50">
+        <v>43587</v>
+      </c>
+      <c r="T38" s="10">
+        <v>60</v>
+      </c>
     </row>
     <row r="39" spans="7:20" x14ac:dyDescent="0.3">
       <c r="G39" s="7" t="s">
@@ -2499,6 +2513,18 @@
       <c r="O39" s="4">
         <v>60</v>
       </c>
+      <c r="Q39" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="R39" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="S39" s="76">
+        <v>43587</v>
+      </c>
+      <c r="T39" s="13">
+        <v>45</v>
+      </c>
     </row>
     <row r="40" spans="7:20" x14ac:dyDescent="0.3">
       <c r="G40" s="10" t="s">
@@ -2525,6 +2551,7 @@
       <c r="O40" s="2">
         <v>30</v>
       </c>
+      <c r="S40" s="32"/>
     </row>
     <row r="41" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L41" s="4" t="s">
@@ -2539,6 +2566,7 @@
       <c r="O41" s="4">
         <v>30</v>
       </c>
+      <c r="S41" s="32"/>
     </row>
     <row r="42" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L42" s="2" t="s">
@@ -2553,6 +2581,7 @@
       <c r="O42" s="2">
         <v>90</v>
       </c>
+      <c r="S42" s="32"/>
     </row>
     <row r="43" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L43" s="4" t="s">
@@ -2567,6 +2596,7 @@
       <c r="O43" s="4">
         <v>50</v>
       </c>
+      <c r="S43" s="32"/>
     </row>
     <row r="44" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L44" s="2" t="s">
@@ -2581,6 +2611,7 @@
       <c r="O44" s="2">
         <v>120</v>
       </c>
+      <c r="S44" s="32"/>
     </row>
     <row r="45" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L45" s="4" t="s">
@@ -2595,6 +2626,7 @@
       <c r="O45" s="4">
         <v>60</v>
       </c>
+      <c r="S45" s="32"/>
     </row>
     <row r="46" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L46" s="2" t="s">
@@ -2737,16 +2769,16 @@
       </c>
     </row>
     <row r="56" spans="12:15" x14ac:dyDescent="0.3">
-      <c r="L56" s="61" t="s">
-        <v>5</v>
-      </c>
-      <c r="M56" s="61" t="s">
+      <c r="L56" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="M56" s="38" t="s">
         <v>16</v>
       </c>
       <c r="N56" s="11">
         <v>43577</v>
       </c>
-      <c r="O56" s="61">
+      <c r="O56" s="38">
         <v>120</v>
       </c>
     </row>
@@ -2759,8 +2791,6 @@
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="J4:Q4"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="G12:J12"/>
     <mergeCell ref="L12:O12"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="B10:C10"/>
@@ -2782,6 +2812,8 @@
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="G12:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update test e tempi
</commit_message>
<xml_diff>
--- a/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_GL3.xlsx
+++ b/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_GL3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Documenti\GitHub\GDPRProject\Documentazione\GDPRPrj_TempiLavoro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gianluca\Documents\GitHub\GDPRProject\Documentazione\GDPRPrj_TempiLavoro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01C28D9-A08F-424F-AE0A-7A5DE7123CAA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D2A93E-C3D5-4143-84AA-36B950FDF144}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="33">
   <si>
     <t>Persona</t>
   </si>
@@ -567,6 +567,31 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -576,7 +601,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -591,21 +631,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -618,31 +643,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -959,94 +959,94 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="T41" sqref="T41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.88671875" customWidth="1"/>
-    <col min="21" max="21" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.85546875" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" customWidth="1"/>
     <col min="22" max="22" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:26" ht="24.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="56" t="s">
+    <row r="1" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:26" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="58"/>
-    </row>
-    <row r="3" spans="2:26" ht="24" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="72"/>
+    </row>
+    <row r="3" spans="2:26" ht="24" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
     </row>
-    <row r="4" spans="2:26" ht="21" x14ac:dyDescent="0.4">
-      <c r="B4" s="60" t="s">
+    <row r="4" spans="2:26" ht="21" x14ac:dyDescent="0.35">
+      <c r="B4" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="62"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="59"/>
       <c r="H4" s="33"/>
-      <c r="J4" s="60" t="s">
+      <c r="J4" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="61"/>
-      <c r="P4" s="61"/>
-      <c r="Q4" s="62"/>
-      <c r="S4" s="75" t="s">
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="58"/>
+      <c r="P4" s="58"/>
+      <c r="Q4" s="59"/>
+      <c r="S4" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="T4" s="75"/>
-      <c r="U4" s="75"/>
-      <c r="V4" s="75"/>
+      <c r="T4" s="55"/>
+      <c r="U4" s="55"/>
+      <c r="V4" s="55"/>
       <c r="W4" s="33"/>
       <c r="X4" s="33"/>
       <c r="Y4" s="33"/>
       <c r="Z4" s="33"/>
     </row>
-    <row r="5" spans="2:26" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:26" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="61"/>
+      <c r="C5" s="58"/>
       <c r="D5" s="29" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="68"/>
-      <c r="G5" s="69"/>
-      <c r="J5" s="74" t="s">
+      <c r="F5" s="64"/>
+      <c r="G5" s="65"/>
+      <c r="J5" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="75"/>
+      <c r="K5" s="55"/>
       <c r="L5" s="34" t="s">
         <v>12</v>
       </c>
@@ -1066,10 +1066,10 @@
         <v>13</v>
       </c>
       <c r="R5" s="41"/>
-      <c r="S5" s="74" t="s">
+      <c r="S5" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="T5" s="75"/>
+      <c r="T5" s="55"/>
       <c r="U5" s="42" t="s">
         <v>10</v>
       </c>
@@ -1077,34 +1077,34 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B6" s="54" t="s">
+    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B6" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="54"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="10">
         <f>SUM(J14:J47)</f>
-        <v>1540</v>
+        <v>1660</v>
       </c>
       <c r="E6" s="27">
         <f t="shared" ref="E6:E8" si="0">_xlfn.FLOOR.MATH(D6/60)</f>
-        <v>25</v>
-      </c>
-      <c r="F6" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="67"/>
-      <c r="J6" s="54" t="s">
+      <c r="G6" s="76"/>
+      <c r="J6" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="54"/>
+      <c r="K6" s="56"/>
       <c r="L6" s="43">
         <f>SUMIF(H14:H47,"CM",J14:J47)</f>
         <v>120</v>
       </c>
       <c r="M6" s="43">
         <f>SUMIF(H14:H47,"Documentazione",J14:J47)</f>
-        <v>1030</v>
+        <v>1090</v>
       </c>
       <c r="N6" s="43">
         <f>SUMIF(H14:H47,"Ricerche",J14:J47)</f>
@@ -1120,26 +1120,26 @@
       </c>
       <c r="Q6" s="43">
         <f>SUMIF(H14:H47,"Test",J14:J47)</f>
-        <v>120</v>
-      </c>
-      <c r="S6" s="54" t="s">
+        <v>180</v>
+      </c>
+      <c r="S6" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="T6" s="54"/>
+      <c r="T6" s="56"/>
       <c r="U6" s="10">
         <f>SUMIF(G14:G48,"Interno",J14:J48)</f>
         <v>240</v>
       </c>
       <c r="V6" s="10">
         <f>SUMIF(G14:G48,"GDPR",J14:J48)</f>
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B7" s="55" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B7" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="55"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="7">
         <f>SUM(O14:O117)</f>
         <v>2850</v>
@@ -1148,14 +1148,14 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="F7" s="64" t="s">
+      <c r="F7" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="65"/>
-      <c r="J7" s="55" t="s">
+      <c r="G7" s="74"/>
+      <c r="J7" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="55"/>
+      <c r="K7" s="69"/>
       <c r="L7" s="44">
         <f>SUMIF(M14:M65,"CM",O14:O65)</f>
         <v>340</v>
@@ -1180,10 +1180,10 @@
         <f>SUMIF(M14:M65,"Test",O14:O65)</f>
         <v>0</v>
       </c>
-      <c r="S7" s="55" t="s">
+      <c r="S7" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="T7" s="55"/>
+      <c r="T7" s="69"/>
       <c r="U7" s="7">
         <f>SUMIF(L14:L68,"Interno",O14:O68)</f>
         <v>400</v>
@@ -1193,11 +1193,11 @@
         <v>2450</v>
       </c>
     </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B8" s="59" t="s">
+    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B8" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="59"/>
+      <c r="C8" s="52"/>
       <c r="D8" s="26">
         <f>SUM(T14:T51)</f>
         <v>2820</v>
@@ -1206,14 +1206,14 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="F8" s="66" t="s">
+      <c r="F8" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="67"/>
-      <c r="J8" s="59" t="s">
+      <c r="G8" s="76"/>
+      <c r="J8" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="59"/>
+      <c r="K8" s="52"/>
       <c r="L8" s="43">
         <f>SUMIF(R14:R47,"CM",T14:T47)</f>
         <v>0</v>
@@ -1238,10 +1238,10 @@
         <f>SUMIF(R14:R47,"Test",T14:T47)</f>
         <v>45</v>
       </c>
-      <c r="S8" s="59" t="s">
+      <c r="S8" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="T8" s="59"/>
+      <c r="T8" s="52"/>
       <c r="U8" s="10">
         <f>SUMIF(Q14:Q48,"Interno",T14:T48)</f>
         <v>0</v>
@@ -1251,11 +1251,11 @@
         <v>2820</v>
       </c>
     </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B9" s="55" t="s">
+    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B9" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="55"/>
+      <c r="C9" s="69"/>
       <c r="D9" s="7">
         <f>SUM(E14:E37)</f>
         <v>750</v>
@@ -1264,24 +1264,24 @@
         <f>_xlfn.FLOOR.MATH(D9/60)*3</f>
         <v>36</v>
       </c>
-      <c r="F9" s="64" t="s">
+      <c r="F9" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="65"/>
+      <c r="G9" s="74"/>
       <c r="H9" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="73" t="s">
+      <c r="J9" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="73"/>
+      <c r="K9" s="53"/>
       <c r="L9" s="45">
         <f>SUMIF(H17:H50,"CM",J17:J50)</f>
         <v>120</v>
       </c>
       <c r="M9" s="45">
         <f>SUM(M6:M8)</f>
-        <v>2945</v>
+        <v>3005</v>
       </c>
       <c r="N9" s="45">
         <f>SUM(N6:N8)</f>
@@ -1297,66 +1297,66 @@
       </c>
       <c r="Q9" s="46">
         <f>SUM(Q6:Q8)</f>
-        <v>165</v>
-      </c>
-      <c r="S9" s="73" t="s">
+        <v>225</v>
+      </c>
+      <c r="S9" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="T9" s="73"/>
+      <c r="T9" s="53"/>
       <c r="U9" s="39">
         <f>SUM(U6:U8)</f>
         <v>640</v>
       </c>
       <c r="V9" s="39">
         <f>SUM(V6:V8)</f>
-        <v>6570</v>
-      </c>
-    </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B10" s="70" t="s">
+        <v>6690</v>
+      </c>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B10" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="70"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="47">
         <f>SUM(D6:D9)</f>
-        <v>7960</v>
+        <v>8080</v>
       </c>
       <c r="E10" s="47">
         <f>SUM(E6:E9)</f>
-        <v>155</v>
-      </c>
-      <c r="F10" s="71" t="s">
+        <v>157</v>
+      </c>
+      <c r="F10" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="72"/>
-    </row>
-    <row r="12" spans="2:26" ht="18" x14ac:dyDescent="0.35">
-      <c r="B12" s="51" t="s">
+      <c r="G10" s="68"/>
+    </row>
+    <row r="12" spans="2:26" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B12" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="53"/>
-      <c r="G12" s="51" t="s">
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="62"/>
+      <c r="G12" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="53"/>
-      <c r="L12" s="51" t="s">
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="62"/>
+      <c r="L12" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="M12" s="52"/>
-      <c r="N12" s="52"/>
-      <c r="O12" s="53"/>
-      <c r="Q12" s="51" t="s">
+      <c r="M12" s="61"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="62"/>
+      <c r="Q12" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="R12" s="52"/>
-      <c r="S12" s="52"/>
-      <c r="T12" s="53"/>
-    </row>
-    <row r="13" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R12" s="61"/>
+      <c r="S12" s="61"/>
+      <c r="T12" s="62"/>
+    </row>
+    <row r="13" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>1</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>5</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>5</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>5</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>5</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>5</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="G25" s="4" t="s">
         <v>5</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="G26" s="2" t="s">
         <v>10</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="G27" s="4" t="s">
         <v>5</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="G28" s="2" t="s">
         <v>5</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="G29" s="4" t="s">
         <v>5</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="G30" s="2" t="s">
         <v>5</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="G31" s="31" t="s">
         <v>5</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="G32" s="38" t="s">
         <v>5</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="7:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G33" s="48" t="s">
         <v>5</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="7:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G34" s="35" t="s">
         <v>5</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="7:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G35" s="37" t="s">
         <v>5</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="36" spans="7:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G36" s="10" t="s">
         <v>10</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="37" spans="7:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G37" s="7" t="s">
         <v>5</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="7:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G38" s="10" t="s">
         <v>5</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="7:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G39" s="7" t="s">
         <v>5</v>
       </c>
@@ -2519,14 +2519,14 @@
       <c r="R39" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="S39" s="76">
+      <c r="S39" s="51">
         <v>43587</v>
       </c>
       <c r="T39" s="13">
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="7:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G40" s="10" t="s">
         <v>5</v>
       </c>
@@ -2553,7 +2553,19 @@
       </c>
       <c r="S40" s="32"/>
     </row>
-    <row r="41" spans="7:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G41" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H41" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I41" s="32">
+        <v>43592</v>
+      </c>
+      <c r="J41" s="12">
+        <v>60</v>
+      </c>
       <c r="L41" s="4" t="s">
         <v>5</v>
       </c>
@@ -2568,7 +2580,19 @@
       </c>
       <c r="S41" s="32"/>
     </row>
-    <row r="42" spans="7:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G42" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I42" s="32">
+        <v>43593</v>
+      </c>
+      <c r="J42" s="15">
+        <v>60</v>
+      </c>
       <c r="L42" s="2" t="s">
         <v>5</v>
       </c>
@@ -2583,7 +2607,7 @@
       </c>
       <c r="S42" s="32"/>
     </row>
-    <row r="43" spans="7:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="7:20" x14ac:dyDescent="0.25">
       <c r="L43" s="4" t="s">
         <v>5</v>
       </c>
@@ -2598,7 +2622,7 @@
       </c>
       <c r="S43" s="32"/>
     </row>
-    <row r="44" spans="7:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="7:20" x14ac:dyDescent="0.25">
       <c r="L44" s="2" t="s">
         <v>5</v>
       </c>
@@ -2613,7 +2637,7 @@
       </c>
       <c r="S44" s="32"/>
     </row>
-    <row r="45" spans="7:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="7:20" x14ac:dyDescent="0.25">
       <c r="L45" s="4" t="s">
         <v>5</v>
       </c>
@@ -2628,7 +2652,7 @@
       </c>
       <c r="S45" s="32"/>
     </row>
-    <row r="46" spans="7:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="7:20" x14ac:dyDescent="0.25">
       <c r="L46" s="2" t="s">
         <v>5</v>
       </c>
@@ -2642,7 +2666,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="7:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="7:20" x14ac:dyDescent="0.25">
       <c r="L47" s="4" t="s">
         <v>5</v>
       </c>
@@ -2656,7 +2680,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="7:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="7:20" x14ac:dyDescent="0.25">
       <c r="L48" s="2" t="s">
         <v>5</v>
       </c>
@@ -2670,7 +2694,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="49" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L49" s="4" t="s">
         <v>10</v>
       </c>
@@ -2684,7 +2708,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L50" s="2" t="s">
         <v>5</v>
       </c>
@@ -2698,7 +2722,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L51" s="4" t="s">
         <v>5</v>
       </c>
@@ -2712,7 +2736,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L52" s="2" t="s">
         <v>5</v>
       </c>
@@ -2726,7 +2750,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L53" s="4" t="s">
         <v>5</v>
       </c>
@@ -2740,7 +2764,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L54" s="2" t="s">
         <v>5</v>
       </c>
@@ -2754,7 +2778,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L55" s="31" t="s">
         <v>5</v>
       </c>
@@ -2768,7 +2792,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L56" s="38" t="s">
         <v>5</v>
       </c>
@@ -2784,20 +2808,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="S4:V4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J4:Q4"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
     <mergeCell ref="Q12:T12"/>
     <mergeCell ref="S6:T6"/>
     <mergeCell ref="S7:T7"/>
@@ -2814,6 +2824,20 @@
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="G12:J12"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="S4:V4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J4:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aggiornato campo date db, modifiche al form per l'aggiunta dell'ora
</commit_message>
<xml_diff>
--- a/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_GL3.xlsx
+++ b/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_GL3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Documents\GitHub\GDPRProject\Documentazione\GDPRPrj_TempiLavoro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Documenti\GitHub\GDPRProject\Documentazione\GDPRPrj_TempiLavoro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AB8970-E78F-44DB-95BC-83A478D4F3B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC58BC74-64B3-4DB0-8AB6-9E391C998BBA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="33">
   <si>
     <t>Persona</t>
   </si>
@@ -567,8 +568,30 @@
     <xf numFmtId="14" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -578,7 +601,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -593,21 +631,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -620,30 +643,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -961,93 +962,93 @@
   <dimension ref="B1:Z59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O61" sqref="O61"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.85546875" customWidth="1"/>
-    <col min="21" max="21" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.88671875" customWidth="1"/>
+    <col min="21" max="21" width="13.44140625" customWidth="1"/>
     <col min="22" max="22" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:26" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="59" t="s">
+    <row r="1" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:26" ht="24.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="61"/>
-    </row>
-    <row r="3" spans="2:26" ht="24" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="72"/>
+    </row>
+    <row r="3" spans="2:26" ht="24" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
     </row>
-    <row r="4" spans="2:26" ht="21" x14ac:dyDescent="0.35">
-      <c r="B4" s="63" t="s">
+    <row r="4" spans="2:26" ht="21" x14ac:dyDescent="0.4">
+      <c r="B4" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="65"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="59"/>
       <c r="H4" s="33"/>
-      <c r="J4" s="63" t="s">
+      <c r="J4" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
-      <c r="O4" s="64"/>
-      <c r="P4" s="64"/>
-      <c r="Q4" s="65"/>
-      <c r="S4" s="78" t="s">
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="58"/>
+      <c r="P4" s="58"/>
+      <c r="Q4" s="59"/>
+      <c r="S4" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="78"/>
+      <c r="T4" s="55"/>
+      <c r="U4" s="55"/>
+      <c r="V4" s="55"/>
       <c r="W4" s="33"/>
       <c r="X4" s="33"/>
       <c r="Y4" s="33"/>
       <c r="Z4" s="33"/>
     </row>
-    <row r="5" spans="2:26" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="66" t="s">
+    <row r="5" spans="2:26" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="64"/>
+      <c r="C5" s="58"/>
       <c r="D5" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="66" t="s">
+      <c r="E5" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="71"/>
-      <c r="G5" s="72"/>
-      <c r="J5" s="77" t="s">
+      <c r="F5" s="64"/>
+      <c r="G5" s="65"/>
+      <c r="J5" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="78"/>
+      <c r="K5" s="55"/>
       <c r="L5" s="34" t="s">
         <v>12</v>
       </c>
@@ -1067,10 +1068,10 @@
         <v>13</v>
       </c>
       <c r="R5" s="41"/>
-      <c r="S5" s="77" t="s">
+      <c r="S5" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="T5" s="78"/>
+      <c r="T5" s="55"/>
       <c r="U5" s="42" t="s">
         <v>10</v>
       </c>
@@ -1078,11 +1079,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B6" s="57" t="s">
+    <row r="6" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B6" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="57"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="10">
         <f>SUM(J14:J47)</f>
         <v>1660</v>
@@ -1091,14 +1092,14 @@
         <f t="shared" ref="E6:E8" si="0">_xlfn.FLOOR.MATH(D6/60)</f>
         <v>27</v>
       </c>
-      <c r="F6" s="69" t="s">
+      <c r="F6" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="70"/>
-      <c r="J6" s="57" t="s">
+      <c r="G6" s="76"/>
+      <c r="J6" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="57"/>
+      <c r="K6" s="56"/>
       <c r="L6" s="43">
         <f>SUMIF(H14:H47,"CM",J14:J47)</f>
         <v>120</v>
@@ -1123,10 +1124,10 @@
         <f>SUMIF(H14:H47,"Test",J14:J47)</f>
         <v>180</v>
       </c>
-      <c r="S6" s="57" t="s">
+      <c r="S6" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="T6" s="57"/>
+      <c r="T6" s="56"/>
       <c r="U6" s="10">
         <f>SUMIF(G14:G48,"Interno",J14:J48)</f>
         <v>240</v>
@@ -1136,11 +1137,11 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B7" s="58" t="s">
+    <row r="7" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B7" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="58"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="7">
         <f>SUM(O14:O117)</f>
         <v>3150</v>
@@ -1149,14 +1150,14 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="F7" s="67" t="s">
+      <c r="F7" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="68"/>
-      <c r="J7" s="58" t="s">
+      <c r="G7" s="74"/>
+      <c r="J7" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="58"/>
+      <c r="K7" s="69"/>
       <c r="L7" s="44">
         <f>SUMIF(M14:M65,"CM",O14:O65)</f>
         <v>340</v>
@@ -1181,10 +1182,10 @@
         <f>SUMIF(M14:M65,"Test",O14:O65)</f>
         <v>0</v>
       </c>
-      <c r="S7" s="58" t="s">
+      <c r="S7" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="T7" s="58"/>
+      <c r="T7" s="69"/>
       <c r="U7" s="7">
         <f>SUMIF(L14:L68,"Interno",O14:O68)</f>
         <v>400</v>
@@ -1194,34 +1195,34 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B8" s="62" t="s">
+    <row r="8" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B8" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="62"/>
+      <c r="C8" s="52"/>
       <c r="D8" s="26">
         <f>SUM(T14:T51)</f>
-        <v>2820</v>
+        <v>3180</v>
       </c>
       <c r="E8" s="27">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="F8" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="70"/>
-      <c r="J8" s="62" t="s">
+      <c r="G8" s="76"/>
+      <c r="J8" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="62"/>
+      <c r="K8" s="52"/>
       <c r="L8" s="43">
         <f>SUMIF(R14:R47,"CM",T14:T47)</f>
         <v>0</v>
       </c>
       <c r="M8" s="43">
         <f>SUMIF(R14:R47,"Documentazione",T14:T47)</f>
-        <v>945</v>
+        <v>1095</v>
       </c>
       <c r="N8" s="43">
         <f>SUMIF(R14:R47,"Ricerche",T14:T47)</f>
@@ -1229,7 +1230,7 @@
       </c>
       <c r="O8" s="43">
         <f>SUMIF(R14:R47,"Codice",T14:T47)</f>
-        <v>1260</v>
+        <v>1470</v>
       </c>
       <c r="P8" s="43">
         <f>SUMIF(R14:R47,"Database",T14:T47)</f>
@@ -1239,24 +1240,24 @@
         <f>SUMIF(R14:R47,"Test",T14:T47)</f>
         <v>45</v>
       </c>
-      <c r="S8" s="62" t="s">
+      <c r="S8" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="T8" s="62"/>
+      <c r="T8" s="52"/>
       <c r="U8" s="10">
         <f>SUMIF(Q14:Q48,"Interno",T14:T48)</f>
         <v>0</v>
       </c>
       <c r="V8" s="10">
         <f>SUMIF(Q14:Q48,"GDPR",T14:T48)</f>
-        <v>2820</v>
-      </c>
-    </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B9" s="58" t="s">
+        <v>3180</v>
+      </c>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B9" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="58"/>
+      <c r="C9" s="69"/>
       <c r="D9" s="7">
         <f>SUM(E14:E37)</f>
         <v>810</v>
@@ -1265,24 +1266,24 @@
         <f>_xlfn.FLOOR.MATH(D9/60)*3</f>
         <v>39</v>
       </c>
-      <c r="F9" s="67" t="s">
+      <c r="F9" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="68"/>
+      <c r="G9" s="74"/>
       <c r="H9" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="76" t="s">
+      <c r="J9" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="76"/>
+      <c r="K9" s="53"/>
       <c r="L9" s="45">
         <f>SUMIF(H17:H50,"CM",J17:J50)</f>
         <v>120</v>
       </c>
       <c r="M9" s="45">
         <f>SUM(M6:M8)</f>
-        <v>3075</v>
+        <v>3225</v>
       </c>
       <c r="N9" s="45">
         <f>SUM(N6:N8)</f>
@@ -1290,7 +1291,7 @@
       </c>
       <c r="O9" s="45">
         <f>SUM(O6:O8)</f>
-        <v>2800</v>
+        <v>3010</v>
       </c>
       <c r="P9" s="46">
         <f>SUM(P6:P8)</f>
@@ -1300,64 +1301,64 @@
         <f>SUM(Q6:Q8)</f>
         <v>225</v>
       </c>
-      <c r="S9" s="76" t="s">
+      <c r="S9" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="T9" s="76"/>
+      <c r="T9" s="53"/>
       <c r="U9" s="39">
         <f>SUM(U6:U8)</f>
         <v>640</v>
       </c>
       <c r="V9" s="39">
         <f>SUM(V6:V8)</f>
-        <v>6990</v>
-      </c>
-    </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B10" s="73" t="s">
+        <v>7350</v>
+      </c>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B10" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="73"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="47">
         <f>SUM(D6:D9)</f>
-        <v>8440</v>
+        <v>8800</v>
       </c>
       <c r="E10" s="47">
         <f>SUM(E6:E9)</f>
-        <v>165</v>
-      </c>
-      <c r="F10" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="F10" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="75"/>
-    </row>
-    <row r="12" spans="2:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="54" t="s">
+      <c r="G10" s="68"/>
+    </row>
+    <row r="12" spans="2:26" ht="18" x14ac:dyDescent="0.35">
+      <c r="B12" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="56"/>
-      <c r="G12" s="54" t="s">
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="62"/>
+      <c r="G12" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="56"/>
-      <c r="L12" s="54" t="s">
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="62"/>
+      <c r="L12" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="M12" s="55"/>
-      <c r="N12" s="55"/>
-      <c r="O12" s="56"/>
-      <c r="Q12" s="54" t="s">
+      <c r="M12" s="61"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="62"/>
+      <c r="Q12" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="R12" s="55"/>
-      <c r="S12" s="55"/>
-      <c r="T12" s="56"/>
-    </row>
-    <row r="13" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R12" s="61"/>
+      <c r="S12" s="61"/>
+      <c r="T12" s="62"/>
+    </row>
+    <row r="13" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
         <v>1</v>
       </c>
@@ -1407,7 +1408,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
@@ -1457,7 +1458,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>5</v>
       </c>
@@ -1507,7 +1508,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
@@ -1557,7 +1558,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
@@ -1607,7 +1608,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
@@ -1657,7 +1658,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
@@ -1707,7 +1708,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>5</v>
       </c>
@@ -1757,7 +1758,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
         <v>5</v>
       </c>
@@ -1807,7 +1808,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
@@ -1857,7 +1858,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>5</v>
       </c>
@@ -1907,17 +1908,17 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="2" t="s">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B24" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="36">
         <v>43558</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="35">
         <v>70</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -1957,17 +1958,17 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B25" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="31" t="s">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B25" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="32">
+      <c r="D25" s="8">
         <v>43593</v>
       </c>
-      <c r="E25" s="31">
+      <c r="E25" s="77">
         <v>60</v>
       </c>
       <c r="G25" s="4" t="s">
@@ -2007,7 +2008,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G26" s="2" t="s">
         <v>10</v>
       </c>
@@ -2045,7 +2046,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G27" s="4" t="s">
         <v>5</v>
       </c>
@@ -2083,7 +2084,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G28" s="2" t="s">
         <v>5</v>
       </c>
@@ -2121,7 +2122,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G29" s="4" t="s">
         <v>5</v>
       </c>
@@ -2159,7 +2160,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G30" s="2" t="s">
         <v>5</v>
       </c>
@@ -2197,7 +2198,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G31" s="31" t="s">
         <v>5</v>
       </c>
@@ -2235,7 +2236,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G32" s="38" t="s">
         <v>5</v>
       </c>
@@ -2273,7 +2274,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:20" x14ac:dyDescent="0.3">
       <c r="G33" s="48" t="s">
         <v>5</v>
       </c>
@@ -2311,7 +2312,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:20" x14ac:dyDescent="0.3">
       <c r="G34" s="35" t="s">
         <v>5</v>
       </c>
@@ -2349,7 +2350,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:20" x14ac:dyDescent="0.3">
       <c r="G35" s="37" t="s">
         <v>5</v>
       </c>
@@ -2387,7 +2388,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="36" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:20" x14ac:dyDescent="0.3">
       <c r="G36" s="10" t="s">
         <v>10</v>
       </c>
@@ -2425,7 +2426,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="37" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:20" x14ac:dyDescent="0.3">
       <c r="G37" s="7" t="s">
         <v>5</v>
       </c>
@@ -2463,7 +2464,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:20" x14ac:dyDescent="0.3">
       <c r="G38" s="10" t="s">
         <v>5</v>
       </c>
@@ -2501,7 +2502,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:20" x14ac:dyDescent="0.3">
       <c r="G39" s="7" t="s">
         <v>5</v>
       </c>
@@ -2539,7 +2540,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:20" x14ac:dyDescent="0.3">
       <c r="G40" s="10" t="s">
         <v>5</v>
       </c>
@@ -2564,19 +2565,30 @@
       <c r="O40" s="2">
         <v>30</v>
       </c>
-      <c r="S40" s="32"/>
-    </row>
-    <row r="41" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G41" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H41" s="12" t="s">
+      <c r="Q40" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="R40" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="S40" s="11">
+        <v>43593</v>
+      </c>
+      <c r="T40" s="10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G41" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="H41" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="I41" s="32">
+      <c r="I41" s="8">
         <v>43592</v>
       </c>
-      <c r="J41" s="12">
+      <c r="J41" s="78">
         <v>60</v>
       </c>
       <c r="L41" s="4" t="s">
@@ -2591,19 +2603,30 @@
       <c r="O41" s="4">
         <v>30</v>
       </c>
-      <c r="S41" s="32"/>
-    </row>
-    <row r="42" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G42" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="H42" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="I42" s="32">
+      <c r="Q41" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="R41" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="S41" s="8">
+        <v>43599</v>
+      </c>
+      <c r="T41" s="13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G42" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I42" s="11">
         <v>43593</v>
       </c>
-      <c r="J42" s="15">
+      <c r="J42" s="10">
         <v>60</v>
       </c>
       <c r="L42" s="2" t="s">
@@ -2618,9 +2641,20 @@
       <c r="O42" s="2">
         <v>90</v>
       </c>
-      <c r="S42" s="32"/>
-    </row>
-    <row r="43" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="Q42" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="R42" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="S42" s="11">
+        <v>43608</v>
+      </c>
+      <c r="T42" s="10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L43" s="4" t="s">
         <v>5</v>
       </c>
@@ -2633,9 +2667,20 @@
       <c r="O43" s="4">
         <v>50</v>
       </c>
-      <c r="S43" s="32"/>
-    </row>
-    <row r="44" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="Q43" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="R43" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="S43" s="8">
+        <v>43609</v>
+      </c>
+      <c r="T43" s="13">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L44" s="2" t="s">
         <v>5</v>
       </c>
@@ -2650,7 +2695,7 @@
       </c>
       <c r="S44" s="32"/>
     </row>
-    <row r="45" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L45" s="4" t="s">
         <v>5</v>
       </c>
@@ -2665,7 +2710,7 @@
       </c>
       <c r="S45" s="32"/>
     </row>
-    <row r="46" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L46" s="2" t="s">
         <v>5</v>
       </c>
@@ -2679,7 +2724,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L47" s="4" t="s">
         <v>5</v>
       </c>
@@ -2693,7 +2738,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="7:20" x14ac:dyDescent="0.3">
       <c r="L48" s="2" t="s">
         <v>5</v>
       </c>
@@ -2707,7 +2752,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="49" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L49" s="4" t="s">
         <v>10</v>
       </c>
@@ -2721,7 +2766,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L50" s="2" t="s">
         <v>5</v>
       </c>
@@ -2735,7 +2780,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L51" s="4" t="s">
         <v>5</v>
       </c>
@@ -2749,7 +2794,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L52" s="2" t="s">
         <v>5</v>
       </c>
@@ -2763,7 +2808,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L53" s="4" t="s">
         <v>5</v>
       </c>
@@ -2777,7 +2822,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L54" s="2" t="s">
         <v>5</v>
       </c>
@@ -2791,7 +2836,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L55" s="31" t="s">
         <v>5</v>
       </c>
@@ -2805,7 +2850,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="12:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L56" s="38" t="s">
         <v>5</v>
       </c>
@@ -2819,64 +2864,50 @@
         <v>120</v>
       </c>
     </row>
-    <row r="57" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L57" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="M57" s="52" t="s">
+    <row r="57" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L57" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="M57" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="N57" s="32">
+      <c r="N57" s="8">
         <v>43593</v>
       </c>
-      <c r="O57" s="52">
+      <c r="O57" s="77">
         <v>140</v>
       </c>
     </row>
-    <row r="58" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L58" s="53" t="s">
-        <v>5</v>
-      </c>
-      <c r="M58" s="53" t="s">
+    <row r="58" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L58" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="M58" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="N58" s="32">
+      <c r="N58" s="11">
         <v>43598</v>
       </c>
-      <c r="O58" s="53">
+      <c r="O58" s="38">
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L59" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="M59" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="N59" s="32">
+    <row r="59" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L59" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="M59" s="77" t="s">
+        <v>11</v>
+      </c>
+      <c r="N59" s="8">
         <v>43608</v>
       </c>
-      <c r="O59" s="52">
+      <c r="O59" s="77">
         <v>70</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="S4:V4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J4:Q4"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
     <mergeCell ref="Q12:T12"/>
     <mergeCell ref="S6:T6"/>
     <mergeCell ref="S7:T7"/>
@@ -2893,6 +2924,20 @@
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="G12:J12"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="S4:V4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J4:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update tempi lucap lucab
</commit_message>
<xml_diff>
--- a/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_GL3.xlsx
+++ b/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_GL3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Documents\GitHub\GDPRProject\Documentazione\GDPRPrj_TempiLavoro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B68569-ADE2-4751-B627-9873CD4BF02C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB75436A-55B0-4842-944A-76D3CE3BC0DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="34">
   <si>
     <t>Persona</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Totali per progetto</t>
+  </si>
+  <si>
+    <t>Migrazione</t>
   </si>
 </sst>
 </file>
@@ -570,9 +573,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -582,70 +649,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -960,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:Z61"/>
+  <dimension ref="B1:Z62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N63" sqref="N63"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,12 +992,12 @@
   <sheetData>
     <row r="1" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:26" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="75"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="63"/>
     </row>
     <row r="3" spans="2:26" ht="24" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B3" s="25"/>
@@ -1003,53 +1006,53 @@
       <c r="E3" s="25"/>
     </row>
     <row r="4" spans="2:26" ht="21" x14ac:dyDescent="0.35">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="62"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="67"/>
       <c r="H4" s="33"/>
-      <c r="J4" s="60" t="s">
+      <c r="J4" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="61"/>
-      <c r="P4" s="61"/>
-      <c r="Q4" s="62"/>
-      <c r="S4" s="58" t="s">
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="67"/>
+      <c r="S4" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="T4" s="58"/>
-      <c r="U4" s="58"/>
-      <c r="V4" s="58"/>
+      <c r="T4" s="80"/>
+      <c r="U4" s="80"/>
+      <c r="V4" s="80"/>
       <c r="W4" s="33"/>
       <c r="X4" s="33"/>
       <c r="Y4" s="33"/>
       <c r="Z4" s="33"/>
     </row>
     <row r="5" spans="2:26" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="61"/>
+      <c r="C5" s="66"/>
       <c r="D5" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="66" t="s">
+      <c r="E5" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="67"/>
-      <c r="G5" s="68"/>
-      <c r="J5" s="57" t="s">
+      <c r="F5" s="73"/>
+      <c r="G5" s="74"/>
+      <c r="J5" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="58"/>
+      <c r="K5" s="80"/>
       <c r="L5" s="34" t="s">
         <v>12</v>
       </c>
@@ -1069,10 +1072,10 @@
         <v>13</v>
       </c>
       <c r="R5" s="41"/>
-      <c r="S5" s="57" t="s">
+      <c r="S5" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="T5" s="58"/>
+      <c r="T5" s="80"/>
       <c r="U5" s="42" t="s">
         <v>10</v>
       </c>
@@ -1093,10 +1096,10 @@
         <f t="shared" ref="E6:E8" si="0">_xlfn.FLOOR.MATH(D6/60)</f>
         <v>27</v>
       </c>
-      <c r="F6" s="78" t="s">
+      <c r="F6" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="79"/>
+      <c r="G6" s="72"/>
       <c r="J6" s="59" t="s">
         <v>14</v>
       </c>
@@ -1139,26 +1142,26 @@
       </c>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="72"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="7">
         <f>SUM(O14:O117)</f>
-        <v>3450</v>
+        <v>3600</v>
       </c>
       <c r="E7" s="28">
         <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="F7" s="76" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="77"/>
-      <c r="J7" s="72" t="s">
+      <c r="G7" s="70"/>
+      <c r="J7" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="72"/>
+      <c r="K7" s="60"/>
       <c r="L7" s="44">
         <f>SUMIF(M14:M65,"CM",O14:O65)</f>
         <v>340</v>
@@ -1183,40 +1186,40 @@
         <f>SUMIF(M14:M65,"Test",O14:O65)</f>
         <v>0</v>
       </c>
-      <c r="S7" s="72" t="s">
+      <c r="S7" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="T7" s="72"/>
+      <c r="T7" s="60"/>
       <c r="U7" s="7">
         <f>SUMIF(L14:L68,"Interno",O14:O68)</f>
         <v>400</v>
       </c>
       <c r="V7" s="7">
         <f>SUMIF(L14:L65,"GDPR",O14:O65)</f>
-        <v>3050</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="55"/>
+      <c r="C8" s="64"/>
       <c r="D8" s="26">
         <f>SUM(T14:T51)</f>
-        <v>3180</v>
+        <v>3330</v>
       </c>
       <c r="E8" s="27">
         <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="F8" s="78" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="79"/>
-      <c r="J8" s="55" t="s">
+      <c r="G8" s="72"/>
+      <c r="J8" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="55"/>
+      <c r="K8" s="64"/>
       <c r="L8" s="43">
         <f>SUMIF(R14:R47,"CM",T14:T47)</f>
         <v>0</v>
@@ -1241,43 +1244,43 @@
         <f>SUMIF(R14:R47,"Test",T14:T47)</f>
         <v>45</v>
       </c>
-      <c r="S8" s="55" t="s">
+      <c r="S8" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="T8" s="55"/>
+      <c r="T8" s="64"/>
       <c r="U8" s="10">
         <f>SUMIF(Q14:Q48,"Interno",T14:T48)</f>
         <v>0</v>
       </c>
       <c r="V8" s="10">
         <f>SUMIF(Q14:Q48,"GDPR",T14:T48)</f>
-        <v>3180</v>
+        <v>3330</v>
       </c>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B9" s="72" t="s">
+      <c r="B9" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="72"/>
+      <c r="C9" s="60"/>
       <c r="D9" s="7">
         <f>SUM(E14:E37)</f>
-        <v>810</v>
+        <v>910</v>
       </c>
       <c r="E9" s="28">
         <f>_xlfn.FLOOR.MATH(D9/60)*3</f>
-        <v>39</v>
-      </c>
-      <c r="F9" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="77"/>
+      <c r="G9" s="70"/>
       <c r="H9" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="56" t="s">
+      <c r="J9" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="56"/>
+      <c r="K9" s="78"/>
       <c r="L9" s="45">
         <f>SUMIF(H17:H50,"CM",J17:J50)</f>
         <v>120</v>
@@ -1302,62 +1305,62 @@
         <f>SUM(Q6:Q8)</f>
         <v>225</v>
       </c>
-      <c r="S9" s="56" t="s">
+      <c r="S9" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="T9" s="56"/>
+      <c r="T9" s="78"/>
       <c r="U9" s="39">
         <f>SUM(U6:U8)</f>
         <v>640</v>
       </c>
       <c r="V9" s="39">
         <f>SUM(V6:V8)</f>
-        <v>7650</v>
+        <v>7950</v>
       </c>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="69"/>
+      <c r="C10" s="75"/>
       <c r="D10" s="47">
         <f>SUM(D6:D9)</f>
-        <v>9100</v>
+        <v>9500</v>
       </c>
       <c r="E10" s="47">
         <f>SUM(E6:E9)</f>
-        <v>176</v>
-      </c>
-      <c r="F10" s="70" t="s">
+        <v>187</v>
+      </c>
+      <c r="F10" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="71"/>
+      <c r="G10" s="77"/>
     </row>
     <row r="12" spans="2:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B12" s="63" t="s">
+      <c r="B12" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="65"/>
-      <c r="G12" s="63" t="s">
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="58"/>
+      <c r="G12" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="64"/>
-      <c r="I12" s="64"/>
-      <c r="J12" s="65"/>
-      <c r="L12" s="63" t="s">
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="58"/>
+      <c r="L12" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="M12" s="64"/>
-      <c r="N12" s="64"/>
-      <c r="O12" s="65"/>
-      <c r="Q12" s="63" t="s">
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
+      <c r="O12" s="58"/>
+      <c r="Q12" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="R12" s="64"/>
-      <c r="S12" s="64"/>
-      <c r="T12" s="65"/>
+      <c r="R12" s="57"/>
+      <c r="S12" s="57"/>
+      <c r="T12" s="58"/>
     </row>
     <row r="13" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
@@ -2010,6 +2013,18 @@
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="32">
+        <v>43635</v>
+      </c>
+      <c r="E26" s="54">
+        <v>100</v>
+      </c>
       <c r="G26" s="2" t="s">
         <v>10</v>
       </c>
@@ -2694,7 +2709,18 @@
       <c r="O44" s="2">
         <v>120</v>
       </c>
-      <c r="S44" s="32"/>
+      <c r="Q44" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="R44" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="S44" s="32">
+        <v>43636</v>
+      </c>
+      <c r="T44" s="15">
+        <v>150</v>
+      </c>
     </row>
     <row r="45" spans="7:20" x14ac:dyDescent="0.25">
       <c r="L45" s="4" t="s">
@@ -2922,21 +2948,49 @@
       </c>
     </row>
     <row r="61" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L61" s="80" t="s">
-        <v>5</v>
-      </c>
-      <c r="M61" s="80" t="s">
+      <c r="L61" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="M61" s="55" t="s">
         <v>16</v>
       </c>
       <c r="N61" s="32">
         <v>43622</v>
       </c>
-      <c r="O61" s="80">
+      <c r="O61" s="55">
         <v>180</v>
+      </c>
+    </row>
+    <row r="62" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L62" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="M62" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="N62" s="32">
+        <v>43636</v>
+      </c>
+      <c r="O62" s="54">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="S4:V4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J4:Q4"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
     <mergeCell ref="Q12:T12"/>
     <mergeCell ref="S6:T6"/>
     <mergeCell ref="S7:T7"/>
@@ -2953,20 +3007,6 @@
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="G12:J12"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="S4:V4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J4:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>